<commit_message>
we got the table finding working - scraping is working time to go for it
</commit_message>
<xml_diff>
--- a/candidates_data.xlsx
+++ b/candidates_data.xlsx
@@ -566,9 +566,21 @@
           <t>None provided</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>August 30, 2023</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
@@ -627,9 +639,21 @@
           <t>None provided</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>May 16, 2016</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
got xls working doing a commit before we do supabase
</commit_message>
<xml_diff>
--- a/candidates_data.xlsx
+++ b/candidates_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,24 +513,20 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Gerecke, Eva</t>
+          <t>,</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9052478</t>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9022278</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9052478</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Eva  Gerecke</t>
-        </is>
-      </c>
+          <t>9022278</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>None</t>
@@ -543,22 +539,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>P.O. Box 1019, 								Sandwich,, 								Massachusetts 02563, 								United States</t>
+          <t>,, 								Outside US and Canada , 								None</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>P.O. Box 106, 								Sagamore,, 								Massachusetts 02561, 								United States</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>7874335505</t>
-        </is>
-      </c>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr">
         <is>
-          <t>evagerecke@gmail.com</t>
+          <t>Maureenwelshfagan@gmail.com</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -568,17 +560,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Master</t>
+          <t>Not Provided</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>None</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>August 30, 2023</t>
+          <t>March 11, 2021</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
@@ -586,75 +578,1389 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Brown-Smalls, Camille</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=5055712</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5055712</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Camille  Brown-Smalls</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>47 Windchime Rd, 								South Easton,, 								Massachusetts 02375, 								United States</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>7814140565</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>csmalls1521@gmail.com</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>July 1, 2023</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Gerecke, Eva</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9052478</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>9052478</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Eva  Gerecke</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>P.O. Box 1019, 								Sandwich,, 								Massachusetts 02563, 								United States</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>P.O. Box 106, 								Sagamore,, 								Massachusetts 02561, 								United States</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>7874335505</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>evagerecke@gmail.com</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>August 30, 2023</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Marshall, Kasondra</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=420051</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>420051</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Kasondra Sporbert  Marshall</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>63 West Otter Drive, 								Tolland,, 								Massachusetts 01034, 								United States</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>413-875-5597</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>ksporber@gmail.com</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>January 1, 2018</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>(Mota) Hutchison, Marissa</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=8355129</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>8355129</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Marissa (Mota) Hutchison</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>489 Turnpike Street APT 5-4, 								South Easton,, 								Massachusetts 02375, 								United States</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>,, 								Massachusetts , 								None</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>5089714956</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>marissavm321@gmail.com</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>August 1, 2023</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>000, 0000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=7774584</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>7774584</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0000 000</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>,, 								Massachusetts , 								United States</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>000-000-0000</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>maryegalvin@gmail.com</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>January 18, 2017</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A, Emma</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=7773464</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7773464</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Emma A</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>76 Perkins St, 								Somerville,, 								Massachusetts 02145, 								United States</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>76 Perkins St, 								Somerville,, 								Massachusetts 02145, 								United States</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>6177970854</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>emmaapplbaum@gmail.com</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>August 28, 2024</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A Hamilton, Samantha</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=6120262</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>6120262</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Samantha Samantha A Hamilton</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>455 Riverside St, 								Lowell,, 								Massachusetts 01854, 								United States</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3392239923</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>samantha.ann.hamilton@gmail.com</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>August 28, 2024</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A Thibeault, Carol</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9145520</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9145520</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Carol Carol A Thibeault</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>146 Fremont St Apt 2, 								Worcester,, 								Massachusetts 01603, 								United States</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>774-418-5466</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>carolthibeault@gmail.com</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Associate</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>July 1, 2023</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Abadie, Melissa</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=101174</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>101174</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Melissa Susan Abadie</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>20 Forest St, 								Taunton,, 								Massachusetts 02780, 								United States</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>20 Forest St, 								Taunton,, 								Massachusetts 02780, 								United States</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>774-526-5779</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>mcote1229@gmail.com</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>August 26, 2024</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Abalos, Teresa</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=10281425</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>10281425</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Teresa Ceblano Abalos</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>B12 L1 P4 St.Scholastica Village, 								Palo,, 								Outside US and Canada 06501, 								Philippines</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>B12 L1 P4 St.Scholastica Village, 								Palo,, 								Outside US and Canada 06501, 								Philippines</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>928-408-2576</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>teresa.abalos001@gmail.com</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>Not provided</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>ABANGAN, MARY JANE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9284073</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>9284073</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>MARY JANE ANASCO ABANGAN</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Na</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Lamac Pinamungajan Cebu, 								Cebu,, 								Outside US and Canada 99999, 								Philippines</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>932-332-2625</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>abanganmj@gmail.com</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>NA</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>June 1, 2023</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Abbay, Setary</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=6620844</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>6620844</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Setary Abbay</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
         <is>
           <t>Actively seeking</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>31 Wood Ave., 								North Andover,, 								Massachusetts 01845, 								United States</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t>,, 								Outside US and Canada , 								None</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>2402533148</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>setbay_biggie@yahoo.com</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K14" t="inlineStr">
         <is>
           <t>None provided</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Bachelor</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
         <is>
           <t>May 16, 2016</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Abbott, Kristen</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=451588</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>451588</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Kristen Abbott</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Abbott</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>35 Lantern Ln., 								Plymouth,, 								Massachusetts 02360, 								United States</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>508-345-8837</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>bumblebeader@gmail.com</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>March 18, 2014</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Abcunas, Leah</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=9092318</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>9092318</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Leah Elizabeth Abcunas</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>201 Cart Path Road, 								Tewksbury,, 								Massachusetts 01876, 								United States</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>,, 								Massachusetts 01876, 								None</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>9784838244</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>leah.abcunas@gmail.com</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>August 5, 2024</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Abdallah, Brian</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=170592</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>170592</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Brian G. Abdallah</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>171 Hinchey Ln, 								Somerset,, 								Massachusetts 02726, 								United States</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>,, 								Massachusetts , 								None</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>5082722188</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>brianabd@comcast.net</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Advanced Studies</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>August 1, 2018</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Abdallah, Jacqueline</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=6840164</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>6840164</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Jacqueline Abdallah</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>801 Ocean Street, 								Marshfield,, 								Massachusetts 02050, 								United States</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>7813080625</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>abdallahjackie@gmail.com</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>January 1, 2017</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Abdelsayed, Mariam</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=3054302</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3054302</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Mariam S Abdelsayed</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Mariam youssef</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>24corning fair banksway , 								westborough,, 								Massachusetts 01581, 								United States</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>5083667085</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>sacredheart38@yahoo.com</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>138</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>September 1, 2014</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Abdul Rahman, Mariama</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=10122748</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>10122748</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Mariama Abdul Rahman</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>230 Abigail Lane, 								Wuakee,, 								Iowa 50263, 								None</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3096128623</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>missabdura24@gmail.com</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Master</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>Not provided</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Abdulkarim, Ainatul Mardia</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://employer.schoolspring.com/employer/pool/candidates/profile.cfm?c_id=10023547</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>10023547</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Ainatul Mardia Abdulatiff Abdulkarim</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Actively seeking</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Phase 2, Country Homes, Ayala, Zamboanga City, Philippines, 								Tausug,, 								Outside US and Canada 70000, 								Philippines</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Phase 2, Country Homes, Ayala, Zamboanga City, Philippines, 								,, 								Outside US and Canada , 								None</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>9976795776</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>ama.abdulkarim08@gmail.com</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>None provided</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Bachelor</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>Not provided</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>